<commit_message>
coordinate pairs of tram1 with some Nan-wrong name
</commit_message>
<xml_diff>
--- a/notebooks/am_tram_routes.xlsx
+++ b/notebooks/am_tram_routes.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A56D40A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A56D4C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A56D4070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A56D4DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A56D4820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58774F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58775B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58776D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58777F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58778B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58779D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5877FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58780D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58781F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58782B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58783D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58784F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58785B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58786D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58787F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58788B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58789D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878D30&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A94BE1C940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94561B400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94EEF3B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94EEF3C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF73A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF77F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF74F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFF7A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C012040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0158B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0157C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0155B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C015BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0283A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0284C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0281C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0281F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C028280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F130&gt;]</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5878E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5878FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58790D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58791F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58792B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58793D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58794F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58795B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58796D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58797F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58798B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58799D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5879FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A1F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A670&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FA90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FDF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68F250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FCD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B68FD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94ADC6AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94ADC6970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94ADC6790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94B996100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94AE34F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00ABB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00A6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C00AE50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0221C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0223D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0223A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0224F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0224C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022910&gt;]</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A587A760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A7F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587A9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AA90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AB50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587ABB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AC10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587ACD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AD30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AD90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587ADF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AE50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AEB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AF10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587AFD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B1F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B7F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587B9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BA90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BB50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BBB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BC10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BCD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BD30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BD90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BDF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BE50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BEB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BF10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587BF70&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A94C0229A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0226D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0227C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0227F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C0225B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94C022F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BA98700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DD95A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DD95970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DD95A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BAEB520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F0FCCD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F0FCD90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F0FCE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F0FCDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F0FCF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F0FCEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFC0D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DD9F670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BFCC2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BA56850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BA56100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DC45FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BA7A100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BA892E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BA89430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F05EF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F05ED90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F05E490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BEE88E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BEE8670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BEE8730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BEE8580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DB8FFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F050F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F050D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F050E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F050FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F050C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F050F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BAA4880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DDAF190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DDAF790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DDAF220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94DDAF5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BE9A0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94BE9A130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F10AA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F10ACA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F10AD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F10A5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F10A5E0&gt;]</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A587E0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E1F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E7F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587E9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EA90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EB50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EBB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EC10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587ECD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587ED30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587ED90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EDF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EE50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EEB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EF10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587EFD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F1F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F7F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587F9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FA90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FB50&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A94F111490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F1116D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F1115E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F1117C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F1118E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F1119A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A94F111FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE00A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE01C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE02E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE03A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE04C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE05E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE06A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE07C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE08E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE09A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE0FA0&gt;]</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A587FC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FCD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FD30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FD90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FDF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FE50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FEB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FF10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A587FFD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58800D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58801F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58802B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58803D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58804F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58805B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58806D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58807F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58808B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58809D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5880FD0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDD9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDDFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC460&gt;]</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5881100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58811F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58812B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58813D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58814F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58815B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58816D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58817F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58818B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58819D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5881FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58820D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58821F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58822B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58823D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58824F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882550&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDC9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EDCFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE20A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE21C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE22E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE23A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE24C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE25E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE26A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE27C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE28E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE29A0&gt;]</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5882640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58826D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58827F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58828B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58829D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5882FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58830D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58831F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58832B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58833D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58834F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58835B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58836D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58837F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58838B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58839D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5883FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58840D0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE2FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE30A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE31C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE32E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE33A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE34C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE35E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE36A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE37C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE38E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE39A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE3FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE40A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE41C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE42E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE43A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE44C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4520&gt;]</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58841C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58841F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58842B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58843D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58844F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58845B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58846D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58847F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58848B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58849D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5884FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58850D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58851F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58852B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58853D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58854F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58855B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58856D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58857F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58858B0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE46A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE47C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE48E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE49A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE4FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE60A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE61C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE62E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE63A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE64C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE65E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE66A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE67C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE68E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE69A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6D00&gt;]</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58859A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58859D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5885FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58860D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58861F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58862B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58863D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58864F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58865B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58866D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58867F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58868B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58869D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886E50&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE6FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE70A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE71C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE72E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE73A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE74C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE75E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE76A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE77C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE78E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE79A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE7FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE80A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE81C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE82E0&gt;]</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5886F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5886FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58880D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58881F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58882B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58883D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58884F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58885B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58886D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58887F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58888B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58889D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5888FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58890D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58891F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58892B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58893D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58894F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58895B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58896D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58897F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58898B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58899D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889A90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889AF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889B50&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EE83D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE84C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE85E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE86A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE87C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE88E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE89A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EE8FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEA9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEABE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEACA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEADC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEAFA0&gt;]</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5889C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889C70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889D90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889DF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889F70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5889FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A1F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A790&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A7F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A850&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588A9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AA30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AA90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AB50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588ABB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AC10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AC70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588ACD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AD30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AD90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588ADF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AE50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AEB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AF10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588AFD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B190&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B1F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B370&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B3D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B430&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B4F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B550&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B5B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B730&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B7F0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B880&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB0D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEB9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEBFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEC9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECCA0&gt;]</t>
         </is>
       </c>
     </row>
@@ -845,7 +845,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A588B970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588B9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588BFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C880&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EECD90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EECFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEE9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEECA0&gt;]</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A588C970&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588C9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588CFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D5E0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EEED90&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEEFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEF9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFA00&gt;]</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A588D6D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588D9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588DFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E3A0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A904EEFFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000000A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000001C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000002E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000003A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000004C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000005E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000006A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000007C0&gt;]</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A588E490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588E9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588ECA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588ED00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588ED60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588EFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588F9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FE80&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A9000008B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000008E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000009A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900000FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000020A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000021C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000022E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000023A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000024C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000025E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000026A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000027C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000028E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000029A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900002FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000030A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000031C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000032E0&gt;]</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A588FF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A588FFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58900A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58901C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58902E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58903A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58904C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58905E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58906A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58907C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58908E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58909A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5890FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58910A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58911C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58912E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58913A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58914C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58915E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58916A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58917C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891820&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A9000033D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000034C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000035E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000036A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000037C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000038E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000039A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900003FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000040A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000041C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000042E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000043A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000044C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000045E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000046A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000047C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000048E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000049A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004C40&gt;]</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5891910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58919A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5891FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58920A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58921C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58922E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58923A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58924C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58925E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58926A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58927C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58928E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58929A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892AC0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900004D30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900004FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000060A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000061C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000062E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000063A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000064C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000065E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000066A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000067C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000068E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000069A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900006EE0&gt;]</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5892BB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5892FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58930A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58931C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58932E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58933A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58934C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58935E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58936A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58937C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58938E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58939A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893DC0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900006FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000070A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000071C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000072E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000073A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000074C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000075E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000076A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000077C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000078E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000079A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900007FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000080A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000081C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008220&gt;]</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5893EB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5893FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58940A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58941C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58942E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58943A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58944C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58945E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58946A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58947C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58948E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58949A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5894FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58950A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58951C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58952E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58953A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58954C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58955E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58956A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58957C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58958E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58959A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895A60&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900008310&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000083A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000084C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000085E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000086A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000087C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000088E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000089A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900008FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000A9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000ABE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000ACA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000ADC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AE80&gt;]</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5895B50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5895FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58960A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58961C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58962E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58963A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58964C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58965E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58966A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58967C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58968E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58969A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5896FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58970A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58971C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58972E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58973A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58974C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58975E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58976A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58977C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897820&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90000AF70&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000AFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000B9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000BFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000C9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CC40&gt;]</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A5897910&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58979A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5897FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58980A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58981C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58982E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58983A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58984C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58985E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58986A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58987C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58988E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58989A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5898FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58990A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58991C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58992E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58993A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58994C0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90000CD30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000CFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000E9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000ECA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000ED00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000ED60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000EFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000F8E0&gt;]</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58995B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58995E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58996A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58997C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58998E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58999A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A5899FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589A9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589ABE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589ACA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589ADC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589AFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B160&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90000F9D0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90000FFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000100A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000101C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000102E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000103A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000104C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000105E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000106A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000107C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000108E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000109A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900010FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000120A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000121C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000122E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000123A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000124C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012580&gt;]</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A589B250&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589B9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589BFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589C9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CAC0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900012670&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000126A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000127C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000128E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000129A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900012FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000130A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000131C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000132E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000133A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000134C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000135E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000136A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000137C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000138E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000139A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900013EE0&gt;]</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A589CBB0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589CFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589D9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589DFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E520&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900013FD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000140A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000141C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000142E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000143A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000144C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000145E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000146A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000147C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000148E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000149A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900014FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000160A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000161C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000162E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000163A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000164C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000165E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000166A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000167C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000168E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016940&gt;]</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A589E610&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589E9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589ECA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589ED00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589ED60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589EFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589F9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FA00&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900016A30&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900016FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000170A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000171C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000172E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000173A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000174C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000175E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000176A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000177C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000178E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000179A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017E20&gt;]</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A589FAF0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A589FFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A00A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A01C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A02E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A03A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A04C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A05E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A06A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A07C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A08E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A09A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0D60&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A900017F10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900017FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000180A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000181C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000182E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000183A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000184C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000185E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000186A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000187C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000188E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A9000189A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A900018FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A1C0&gt;]</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0E50&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A0FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A10A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A11C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A12E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A13A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A14C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A15E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A16A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A17C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A18E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A19A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A1FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A20A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A21C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A22E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A23A0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90001A2B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001A9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001ABE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001ACA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001ADC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001AFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B7C0&gt;]</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2490&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A24C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A25E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A26A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A27C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A28E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A29A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2BE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A2FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A30A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A31C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A32E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A33A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A34C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A35E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A36A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A37C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A38E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A39A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3B20&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90001B8B0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001B9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001BFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001C9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001CF40&gt;]</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3C10&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3C40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3CA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A3FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A40A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A41C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A42E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A43A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A44C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A45E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A46A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A47C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A48E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A49A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4B20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4B80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4BE0&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90001E070&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E0A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001E9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001ECA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001ED00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001ED60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EF40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001EFA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F040&gt;]</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[&lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4CD0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4D00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4D60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4DC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4E20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4E80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4EE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4F40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A4FA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5040&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A50A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5100&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A51C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A52E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A53A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A54C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A55E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A56A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A57C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A58E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A59A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5A00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5A60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5AC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x00000272A58A5B20&gt;]</t>
+          <t>[&lt;shapely.geometry.linestring.LineString object at 0x000002A90001F130&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F160&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F1C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F220&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F280&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F2E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F340&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F3A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F400&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F460&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F4C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F520&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F580&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F5E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F640&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F6A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F700&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F760&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F7C0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F820&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F880&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F8E0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F940&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001F9A0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FA00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FA60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FAC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FB20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FB80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FBE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FC40&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FCA0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FD00&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FD60&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FDC0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FE20&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FE80&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FEE0&gt;, &lt;shapely.geometry.linestring.LineString object at 0x000002A90001FF40&gt;]</t>
         </is>
       </c>
     </row>

</xml_diff>